<commit_message>
memory efficient implementation of masking preprocessing
</commit_message>
<xml_diff>
--- a/training.xlsx
+++ b/training.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gapaza/repos/gabe/hydra-chess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D909127-2E6B-234E-9043-2BB472B80738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA58881-B7B7-3D42-8056-AFE6256E1C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{BBDF2B30-CE7A-5D41-817F-FBBDD73D7D69}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{BBDF2B30-CE7A-5D41-817F-FBBDD73D7D69}"/>
   </bookViews>
   <sheets>
     <sheet name="Pretraining" sheetId="1" r:id="rId1"/>
+    <sheet name="Pretraining Med (1mil)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,25 +37,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
-    <t>Move Validation (3 encoders, 100k)</t>
+    <t>Move Validation
+ (3 encoders, 100k)</t>
   </si>
   <si>
-    <t>Board Validation (3 encoders, 100k)</t>
+    <t>Board Validation 
+(3 encoders, 100k)</t>
   </si>
   <si>
-    <t>Move Validation (3 encoders, 200k)</t>
+    <t>Move Validation 
+(3 encoders, 200k)</t>
   </si>
   <si>
-    <t>Board Validation (3 encoders, 200k)</t>
+    <t>Board Validation 
+(3 encoders, 200k)</t>
+  </si>
+  <si>
+    <t>Move Validation 
+(3 encoders, 100k, No SPT)</t>
+  </si>
+  <si>
+    <t>Board Validation 
+(3 encoders, 100k, no SPT)</t>
+  </si>
+  <si>
+    <t>Move Validation 
+(3 encoders, 100k, No SPT, pad)</t>
+  </si>
+  <si>
+    <t>Board Validation 
+(3 encoders, 100k, no SPT, pad)</t>
+  </si>
+  <si>
+    <t>Specs: 
+2048 dense dim, 3 encoders, 256 embed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move Validation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board Validation </t>
+  </si>
+  <si>
+    <t>Notes: best paraters are
+30% board masking
+no shifted patch tokenization</t>
+  </si>
+  <si>
+    <t>Specs: 
+2048 dense dim, 5 encoders, 256 embed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -62,13 +102,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D08E"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,12 +148,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,73 +490,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6C4619-DC3A-8144-9EEE-1E48AF343753}">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="B1" zoomScale="102" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="30.1640625" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" customWidth="1"/>
-    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="1" max="1" width="38" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.83203125" customWidth="1"/>
+    <col min="16" max="16" width="19.33203125" customWidth="1"/>
+    <col min="17" max="17" width="27.83203125" customWidth="1"/>
+    <col min="18" max="18" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="L1" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M1" t="s">
+      <c r="L1" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="N1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0.2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.25</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>0.2</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>0.25</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0.3</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>0.4</v>
       </c>
-      <c r="L2" s="2">
+      <c r="K2" s="1">
         <v>0.3</v>
       </c>
-      <c r="M2" s="2">
+      <c r="L2" s="1">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4.8300000000000003E-2</v>
       </c>
@@ -494,14 +614,26 @@
       <c r="I3">
         <v>0.74309999999999998</v>
       </c>
+      <c r="K3">
+        <v>6.9500000000000006E-2</v>
+      </c>
       <c r="L3">
-        <v>6.9500000000000006E-2</v>
-      </c>
-      <c r="M3">
         <v>0.76880000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="O3">
+        <v>0.75519999999999998</v>
+      </c>
+      <c r="Q3">
+        <v>5.4699999999999999E-2</v>
+      </c>
+      <c r="R3">
+        <v>0.75829999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6.88E-2</v>
       </c>
@@ -526,14 +658,26 @@
       <c r="I4">
         <v>0.77569999999999995</v>
       </c>
+      <c r="K4">
+        <v>0.1215</v>
+      </c>
       <c r="L4">
-        <v>0.1215</v>
-      </c>
-      <c r="M4">
         <v>0.80710000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="O4">
+        <v>0.78210000000000002</v>
+      </c>
+      <c r="Q4">
+        <v>8.8800000000000004E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.78349999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8.8400000000000006E-2</v>
       </c>
@@ -558,14 +702,26 @@
       <c r="I5">
         <v>0.79900000000000004</v>
       </c>
+      <c r="K5">
+        <v>0.1711</v>
+      </c>
       <c r="L5">
-        <v>0.1711</v>
-      </c>
-      <c r="M5">
         <v>0.83309999999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="O5">
+        <v>0.79949999999999999</v>
+      </c>
+      <c r="Q5">
+        <v>0.13370000000000001</v>
+      </c>
+      <c r="R5">
+        <v>0.80049999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.1099</v>
       </c>
@@ -590,8 +746,26 @@
       <c r="I6">
         <v>0.81789999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0.20849999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.85009999999999997</v>
+      </c>
+      <c r="N6">
+        <v>0.15440000000000001</v>
+      </c>
+      <c r="O6">
+        <v>0.81210000000000004</v>
+      </c>
+      <c r="Q6">
+        <v>0.1736</v>
+      </c>
+      <c r="R6">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.13200000000000001</v>
       </c>
@@ -616,8 +790,26 @@
       <c r="I7">
         <v>0.83220000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>0.23419999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="N7">
+        <v>0.17630000000000001</v>
+      </c>
+      <c r="O7">
+        <v>0.82179999999999997</v>
+      </c>
+      <c r="Q7">
+        <v>0.20019999999999999</v>
+      </c>
+      <c r="R7">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.1565</v>
       </c>
@@ -642,8 +834,26 @@
       <c r="I8">
         <v>0.84309999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0.2601</v>
+      </c>
+      <c r="L8">
+        <v>0.87109999999999999</v>
+      </c>
+      <c r="N8">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="O8">
+        <v>0.82969999999999999</v>
+      </c>
+      <c r="Q8">
+        <v>0.22439999999999999</v>
+      </c>
+      <c r="R8">
+        <v>0.82989999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.1769</v>
       </c>
@@ -668,8 +878,26 @@
       <c r="I9">
         <v>0.85170000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>0.28310000000000002</v>
+      </c>
+      <c r="L9">
+        <v>0.87829999999999997</v>
+      </c>
+      <c r="N9">
+        <v>0.22309999999999999</v>
+      </c>
+      <c r="O9">
+        <v>0.83620000000000005</v>
+      </c>
+      <c r="Q9">
+        <v>0.24129999999999999</v>
+      </c>
+      <c r="R9">
+        <v>0.83679999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.19689999999999999</v>
       </c>
@@ -694,8 +922,26 @@
       <c r="I10">
         <v>0.85870000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>0.30509999999999998</v>
+      </c>
+      <c r="L10">
+        <v>0.88419999999999999</v>
+      </c>
+      <c r="N10">
+        <v>0.2394</v>
+      </c>
+      <c r="O10">
+        <v>0.84179999999999999</v>
+      </c>
+      <c r="Q10">
+        <v>0.2571</v>
+      </c>
+      <c r="R10">
+        <v>0.84279999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.215</v>
       </c>
@@ -714,8 +960,26 @@
       <c r="H11">
         <v>0.85699999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>0.32379999999999998</v>
+      </c>
+      <c r="L11">
+        <v>0.88919999999999999</v>
+      </c>
+      <c r="N11">
+        <v>0.25009999999999999</v>
+      </c>
+      <c r="O11">
+        <v>0.84650000000000003</v>
+      </c>
+      <c r="Q11">
+        <v>0.27360000000000001</v>
+      </c>
+      <c r="R11">
+        <v>0.84809999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.2281</v>
       </c>
@@ -734,8 +998,26 @@
       <c r="H12">
         <v>0.86219999999999997</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>0.34229999999999999</v>
+      </c>
+      <c r="L12">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="N12">
+        <v>0.2586</v>
+      </c>
+      <c r="O12">
+        <v>0.85050000000000003</v>
+      </c>
+      <c r="Q12">
+        <v>0.28189999999999998</v>
+      </c>
+      <c r="R12">
+        <v>0.85289999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>0.21640000000000001</v>
       </c>
@@ -749,7 +1031,7 @@
         <v>0.86660000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>0.22120000000000001</v>
       </c>
@@ -757,12 +1039,17 @@
         <v>0.84850000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>0.2225</v>
       </c>
       <c r="G15">
         <v>0.85289999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -772,4 +1059,155 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30EC8A22-87AB-1543-9AEB-D8C279941D5B}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="12">
+        <v>0.36809999999999998</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0.85840000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="11">
+        <v>0.53269999999999995</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.89639999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="11">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="C4" s="11">
+        <v>0.91510000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+    </row>
+    <row r="11" spans="1:3" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="11">
+        <v>0.29110000000000003</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0.83640000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>0.40179999999999999</v>
+      </c>
+      <c r="C13">
+        <v>0.86719999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>0.49320000000000003</v>
+      </c>
+      <c r="C14">
+        <v>0.88580000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>0.57240000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.89959999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0.624</v>
+      </c>
+      <c r="C16">
+        <v>0.91020000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>0.69240000000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.91890000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>0.76970000000000005</v>
+      </c>
+      <c r="C18">
+        <v>0.92630000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="11">
+        <v>0.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>